<commit_message>
Add chart for CMA Cohen's Kappa
</commit_message>
<xml_diff>
--- a/study/data/stats/combined/stats-combined-classification-agreement.xlsx
+++ b/study/data/stats/combined/stats-combined-classification-agreement.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="4728" windowWidth="46128" windowHeight="17436"/>
+    <workbookView xWindow="-12" yWindow="4728" windowWidth="46128" windowHeight="17436" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="POCMA" sheetId="2" r:id="rId1"/>
     <sheet name="CKFCMA" sheetId="5" r:id="rId2"/>
     <sheet name="POCMA TS" sheetId="4" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <definedNames>
     <definedName name="ADAM_ALL">#REF!</definedName>
     <definedName name="ALLALL_CK">CKFCMA!$N$6</definedName>
@@ -540,6 +543,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -548,9 +554,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -562,6 +565,307 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:style val="1"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l">
+              <a:defRPr sz="1800">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Cohen's Kappa</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> for Manual Classification Agreement</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.456719644608396E-2"/>
+          <c:y val="3.9808760654034853E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inBase"/>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>CKFCMA!$A$6:$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>ALL</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>urgency</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>work-logistics</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>work-pers</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>interested</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>work-relevant</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>company-law</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>cycling</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>cycling-logistics</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>football</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>friend-group</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>golf</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>golf-logistics</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>pers-urgency</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>personal-interested</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>riding</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>riding-arrangements</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>school-importance</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>tech</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>tennis</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>tennis-arrangements</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>tennis-organising</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>work-urgency</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CKFCMA!$N$6:$N$29</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0.83599999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78033333333333343</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.67300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.73733333333333329</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.72366666666666679</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.55500000000000005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.79100000000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.86699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.54900000000000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.748</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.76500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.47499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.50600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.30599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.64200000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="55"/>
+        <c:overlap val="-7"/>
+        <c:axId val="189073664"/>
+        <c:axId val="189076992"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="189073664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000">
+                <a:latin typeface="Courier New" pitchFamily="49" charset="0"/>
+                <a:cs typeface="Courier New" pitchFamily="49" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="189076992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="189076992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="189073664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-GB"/>
   <c:chart>
@@ -633,24 +937,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="119805056"/>
-        <c:axId val="119806592"/>
+        <c:axId val="120591488"/>
+        <c:axId val="120593024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="119805056"/>
+        <c:axId val="120591488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119806592"/>
+        <c:crossAx val="120593024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="119806592"/>
+        <c:axId val="120593024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -658,7 +962,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119805056"/>
+        <c:crossAx val="120591488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -667,13 +971,48 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>990600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -706,6 +1045,102 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="PFEF SRC"/>
+      <sheetName val="PFEF T"/>
+      <sheetName val="PFEF C"/>
+      <sheetName val="PFEA SRC"/>
+      <sheetName val="PFEA T"/>
+      <sheetName val="PFEA C"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="7">
+          <cell r="B7" t="str">
+            <v>ALL</v>
+          </cell>
+          <cell r="U7">
+            <v>0.37723877925437943</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v>interested</v>
+          </cell>
+          <cell r="U8">
+            <v>0.50416661987288003</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>tennis</v>
+          </cell>
+          <cell r="U9">
+            <v>0.58385827500163889</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>tennis-arrangements</v>
+          </cell>
+          <cell r="U10">
+            <v>0.29386188653629097</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11" t="str">
+            <v>tennis-organising</v>
+          </cell>
+          <cell r="U11">
+            <v>0.57928848262966048</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12" t="str">
+            <v>urgency</v>
+          </cell>
+          <cell r="U12">
+            <v>0.57149971405294531</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13" t="str">
+            <v>work-logistics</v>
+          </cell>
+          <cell r="U13">
+            <v>0.73538675494728178</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="B14" t="str">
+            <v>work-pers</v>
+          </cell>
+          <cell r="U14">
+            <v>0.67835317926251881</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15" t="str">
+            <v>work-relevant</v>
+          </cell>
+          <cell r="U15">
+            <v>0.45285214433040366</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -998,7 +1433,7 @@
   </sheetPr>
   <dimension ref="A1:AC34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AH40" sqref="AH40"/>
     </sheetView>
   </sheetViews>
@@ -1065,73 +1500,73 @@
       <c r="AC2" s="29"/>
     </row>
     <row r="3" spans="1:29" ht="52.2" customHeight="1">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="53"/>
-      <c r="T3" s="53"/>
-      <c r="U3" s="53"/>
-      <c r="V3" s="53"/>
-      <c r="W3" s="53"/>
-      <c r="X3" s="53"/>
-      <c r="Y3" s="53"/>
-      <c r="Z3" s="53"/>
-      <c r="AA3" s="53"/>
-      <c r="AB3" s="53"/>
-      <c r="AC3" s="53"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="54"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="54"/>
+      <c r="Y3" s="54"/>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="54"/>
+      <c r="AB3" s="54"/>
+      <c r="AC3" s="54"/>
     </row>
     <row r="4" spans="1:29" s="16" customFormat="1">
       <c r="A4" s="25"/>
       <c r="B4" s="18"/>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="H4" s="54" t="s">
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="H4" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="L4" s="54" t="s">
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="L4" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54"/>
+      <c r="M4" s="55"/>
+      <c r="N4" s="55"/>
       <c r="O4" s="18"/>
-      <c r="P4" s="54" t="s">
+      <c r="P4" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="54"/>
+      <c r="Q4" s="55"/>
+      <c r="R4" s="55"/>
       <c r="S4" s="18"/>
-      <c r="T4" s="54" t="s">
+      <c r="T4" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="U4" s="54"/>
-      <c r="V4" s="54"/>
-      <c r="X4" s="54" t="s">
+      <c r="U4" s="55"/>
+      <c r="V4" s="55"/>
+      <c r="X4" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="Y4" s="54"/>
-      <c r="Z4" s="54"/>
+      <c r="Y4" s="55"/>
+      <c r="Z4" s="55"/>
       <c r="AA4" s="15"/>
       <c r="AC4" s="29"/>
     </row>
@@ -2477,8 +2912,8 @@
   </sheetPr>
   <dimension ref="A1:AC49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V32" sqref="V32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W49" sqref="W49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2497,7 +2932,7 @@
     <col min="12" max="12" width="8.21875" style="35" customWidth="1"/>
     <col min="13" max="13" width="1.44140625" customWidth="1"/>
     <col min="14" max="14" width="8.21875" style="37" customWidth="1"/>
-    <col min="15" max="15" width="5.77734375" style="56" customWidth="1"/>
+    <col min="15" max="15" width="5.77734375" style="53" customWidth="1"/>
     <col min="16" max="16" width="1.109375" customWidth="1"/>
     <col min="17" max="17" width="4.6640625" style="29" customWidth="1"/>
   </cols>
@@ -2521,29 +2956,29 @@
       <c r="K2" s="18"/>
       <c r="L2" s="33"/>
       <c r="N2" s="38"/>
-      <c r="O2" s="56"/>
+      <c r="O2" s="53"/>
       <c r="Q2" s="29"/>
     </row>
     <row r="3" spans="1:29" ht="97.8" customHeight="1">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
       <c r="R3" s="43"/>
       <c r="S3" s="43"/>
       <c r="T3" s="43"/>
@@ -2584,7 +3019,7 @@
       <c r="N4" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="56"/>
+      <c r="O4" s="53"/>
       <c r="Q4" s="30"/>
     </row>
     <row r="5" spans="1:29" s="21" customFormat="1" ht="6" customHeight="1">
@@ -2598,7 +3033,7 @@
       <c r="K5" s="22"/>
       <c r="L5" s="34"/>
       <c r="N5" s="39"/>
-      <c r="O5" s="56"/>
+      <c r="O5" s="53"/>
       <c r="Q5" s="30"/>
     </row>
     <row r="6" spans="1:29" s="16" customFormat="1">
@@ -2622,7 +3057,7 @@
         <f>(D6+F6+J6)/3</f>
         <v>0.83599999999999997</v>
       </c>
-      <c r="O6" s="56"/>
+      <c r="O6" s="53"/>
       <c r="Q6" s="29" t="s">
         <v>10</v>
       </c>
@@ -2636,7 +3071,7 @@
       <c r="K7" s="18"/>
       <c r="L7" s="33"/>
       <c r="N7" s="38"/>
-      <c r="O7" s="56"/>
+      <c r="O7" s="53"/>
       <c r="Q7" s="29"/>
     </row>
     <row r="8" spans="1:29" s="16" customFormat="1">
@@ -2662,7 +3097,7 @@
         <f>(D8+F8+J8)/3</f>
         <v>0.78033333333333343</v>
       </c>
-      <c r="O8" s="56">
+      <c r="O8" s="53">
         <f t="shared" ref="O8:O29" si="0">N8-ALLALL_CK</f>
         <v>-5.5666666666666531E-2</v>
       </c>
@@ -2693,7 +3128,7 @@
         <f>(D9+F9+J9)/3</f>
         <v>0.67300000000000004</v>
       </c>
-      <c r="O9" s="56">
+      <c r="O9" s="53">
         <f t="shared" si="0"/>
         <v>-0.16299999999999992</v>
       </c>
@@ -2724,7 +3159,7 @@
         <f>(D10+F10+J10)/3</f>
         <v>0.73733333333333329</v>
       </c>
-      <c r="O10" s="56">
+      <c r="O10" s="53">
         <f t="shared" si="0"/>
         <v>-9.866666666666668E-2</v>
       </c>
@@ -2755,7 +3190,7 @@
         <f>(D11+F11+J11)/3</f>
         <v>0.72366666666666679</v>
       </c>
-      <c r="O11" s="56">
+      <c r="O11" s="53">
         <f t="shared" si="0"/>
         <v>-0.11233333333333317</v>
       </c>
@@ -2784,7 +3219,7 @@
         <f>(D12+F12+J12)/2</f>
         <v>0.23100000000000001</v>
       </c>
-      <c r="O12" s="56">
+      <c r="O12" s="53">
         <f t="shared" si="0"/>
         <v>-0.60499999999999998</v>
       </c>
@@ -2809,7 +3244,7 @@
         <f t="shared" ref="N13:N19" si="1">(D13+F13+J13)/B13</f>
         <v>0</v>
       </c>
-      <c r="O13" s="56">
+      <c r="O13" s="53">
         <f t="shared" si="0"/>
         <v>-0.83599999999999997</v>
       </c>
@@ -2836,7 +3271,7 @@
         <f t="shared" si="1"/>
         <v>0.79</v>
       </c>
-      <c r="O14" s="56">
+      <c r="O14" s="53">
         <f t="shared" si="0"/>
         <v>-4.599999999999993E-2</v>
       </c>
@@ -2863,7 +3298,7 @@
         <f t="shared" si="1"/>
         <v>0.55500000000000005</v>
       </c>
-      <c r="O15" s="56">
+      <c r="O15" s="53">
         <f t="shared" si="0"/>
         <v>-0.28099999999999992</v>
       </c>
@@ -2890,7 +3325,7 @@
         <f t="shared" si="1"/>
         <v>0.79100000000000004</v>
       </c>
-      <c r="O16" s="56">
+      <c r="O16" s="53">
         <f t="shared" si="0"/>
         <v>-4.4999999999999929E-2</v>
       </c>
@@ -2915,7 +3350,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O17" s="56">
+      <c r="O17" s="53">
         <f t="shared" si="0"/>
         <v>-0.83599999999999997</v>
       </c>
@@ -2942,7 +3377,7 @@
         <f t="shared" si="1"/>
         <v>0.86699999999999999</v>
       </c>
-      <c r="O18" s="56">
+      <c r="O18" s="53">
         <f t="shared" si="0"/>
         <v>3.1000000000000028E-2</v>
       </c>
@@ -2969,7 +3404,7 @@
         <f t="shared" si="1"/>
         <v>0.54900000000000004</v>
       </c>
-      <c r="O19" s="56">
+      <c r="O19" s="53">
         <f t="shared" si="0"/>
         <v>-0.28699999999999992</v>
       </c>
@@ -2997,7 +3432,7 @@
         <f t="shared" ref="N20:N29" si="2">(D20+F20+H20)/B20</f>
         <v>0.748</v>
       </c>
-      <c r="O20" s="56">
+      <c r="O20" s="53">
         <f t="shared" si="0"/>
         <v>-8.7999999999999967E-2</v>
       </c>
@@ -3023,7 +3458,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O21" s="56">
+      <c r="O21" s="53">
         <f t="shared" si="0"/>
         <v>-0.83599999999999997</v>
       </c>
@@ -3049,7 +3484,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O22" s="56">
+      <c r="O22" s="53">
         <f t="shared" si="0"/>
         <v>-0.83599999999999997</v>
       </c>
@@ -3075,7 +3510,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O23" s="56">
+      <c r="O23" s="53">
         <f t="shared" si="0"/>
         <v>-0.83599999999999997</v>
       </c>
@@ -3101,7 +3536,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O24" s="56">
+      <c r="O24" s="53">
         <f t="shared" si="0"/>
         <v>-0.83599999999999997</v>
       </c>
@@ -3129,7 +3564,7 @@
         <f t="shared" si="2"/>
         <v>0.76500000000000001</v>
       </c>
-      <c r="O25" s="56">
+      <c r="O25" s="53">
         <f t="shared" si="0"/>
         <v>-7.0999999999999952E-2</v>
       </c>
@@ -3157,7 +3592,7 @@
         <f t="shared" si="2"/>
         <v>0.47499999999999998</v>
       </c>
-      <c r="O26" s="56">
+      <c r="O26" s="53">
         <f t="shared" si="0"/>
         <v>-0.36099999999999999</v>
       </c>
@@ -3185,7 +3620,7 @@
         <f t="shared" si="2"/>
         <v>0.50600000000000001</v>
       </c>
-      <c r="O27" s="56">
+      <c r="O27" s="53">
         <f t="shared" si="0"/>
         <v>-0.32999999999999996</v>
       </c>
@@ -3213,7 +3648,7 @@
         <f t="shared" si="2"/>
         <v>0.30599999999999999</v>
       </c>
-      <c r="O28" s="56">
+      <c r="O28" s="53">
         <f t="shared" si="0"/>
         <v>-0.53</v>
       </c>
@@ -3241,7 +3676,7 @@
         <f t="shared" si="2"/>
         <v>0.64200000000000002</v>
       </c>
-      <c r="O29" s="56">
+      <c r="O29" s="53">
         <f t="shared" si="0"/>
         <v>-0.19399999999999995</v>
       </c>
@@ -3260,7 +3695,7 @@
       <c r="K30" s="18"/>
       <c r="L30" s="33"/>
       <c r="N30" s="38"/>
-      <c r="O30" s="56"/>
+      <c r="O30" s="53"/>
       <c r="Q30" s="29"/>
     </row>
     <row r="31" spans="1:17">
@@ -3290,7 +3725,7 @@
       <c r="L33" s="35"/>
       <c r="M33"/>
       <c r="N33" s="40"/>
-      <c r="O33" s="56"/>
+      <c r="O33" s="53"/>
       <c r="P33"/>
       <c r="Q33" s="29"/>
     </row>
@@ -3309,7 +3744,7 @@
       <c r="L34" s="35"/>
       <c r="M34"/>
       <c r="N34" s="40"/>
-      <c r="O34" s="56"/>
+      <c r="O34" s="53"/>
       <c r="P34"/>
       <c r="Q34" s="29"/>
     </row>
@@ -3351,7 +3786,8 @@
     <mergeCell ref="A3:Q3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="94" fitToWidth="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToWidth="0" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3401,69 +3837,69 @@
     </row>
     <row r="2" spans="1:29" ht="7.2" customHeight="1"/>
     <row r="3" spans="1:29" ht="49.8" customHeight="1">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="53"/>
-      <c r="T3" s="53"/>
-      <c r="U3" s="53"/>
-      <c r="V3" s="53"/>
-      <c r="W3" s="53"/>
-      <c r="X3" s="53"/>
-      <c r="Y3" s="53"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="54"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="54"/>
+      <c r="Y3" s="54"/>
       <c r="Z3" s="43"/>
       <c r="AA3" s="43"/>
       <c r="AB3" s="43"/>
       <c r="AC3" s="43"/>
     </row>
     <row r="4" spans="1:29">
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="G4" s="55" t="s">
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="G4" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="K4" s="55" t="s">
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="K4" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="L4" s="55"/>
-      <c r="M4" s="55"/>
-      <c r="O4" s="55" t="s">
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="O4" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="55"/>
-      <c r="Q4" s="55"/>
-      <c r="S4" s="55" t="s">
+      <c r="P4" s="56"/>
+      <c r="Q4" s="56"/>
+      <c r="S4" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="T4" s="55"/>
-      <c r="U4" s="55"/>
-      <c r="W4" s="55" t="s">
+      <c r="T4" s="56"/>
+      <c r="U4" s="56"/>
+      <c r="W4" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="55"/>
-      <c r="Y4" s="55"/>
+      <c r="X4" s="56"/>
+      <c r="Y4" s="56"/>
     </row>
     <row r="5" spans="1:29" s="1" customFormat="1">
       <c r="A5" s="1" t="s">

</xml_diff>

<commit_message>
Change time series chart format to line
</commit_message>
<xml_diff>
--- a/study/data/stats/combined/stats-combined-classification-agreement.xlsx
+++ b/study/data/stats/combined/stats-combined-classification-agreement.xlsx
@@ -4,16 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="4728" windowWidth="46128" windowHeight="17436" activeTab="1"/>
+    <workbookView xWindow="-12" yWindow="4728" windowWidth="46128" windowHeight="17436" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="POCMA" sheetId="2" r:id="rId1"/>
     <sheet name="CKFCMA" sheetId="5" r:id="rId2"/>
     <sheet name="POCMA TS" sheetId="4" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="ADAM_ALL">#REF!</definedName>
     <definedName name="ALLALL_CK">CKFCMA!$N$6</definedName>
@@ -622,7 +619,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.456719644608396E-2"/>
+          <c:x val="5.4567196446083981E-2"/>
           <c:y val="3.9808760654034853E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -812,11 +809,11 @@
         </c:ser>
         <c:gapWidth val="55"/>
         <c:overlap val="-7"/>
-        <c:axId val="189073664"/>
-        <c:axId val="189076992"/>
+        <c:axId val="127212928"/>
+        <c:axId val="127227008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="189073664"/>
+        <c:axId val="127212928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -835,14 +832,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189076992"/>
+        <c:crossAx val="127227008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189076992"/>
+        <c:axId val="127227008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -850,7 +847,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189073664"/>
+        <c:crossAx val="127212928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -859,7 +856,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -877,6 +874,14 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
           <c:cat>
             <c:strRef>
               <c:f>'POCMA TS'!$A$7:$A$13</c:f>
@@ -937,24 +942,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="120591488"/>
-        <c:axId val="120593024"/>
+        <c:axId val="127241216"/>
+        <c:axId val="127759104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="120591488"/>
+        <c:axId val="127241216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120593024"/>
+        <c:crossAx val="127759104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="120593024"/>
+        <c:axId val="127759104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -962,7 +967,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120591488"/>
+        <c:crossAx val="127241216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -971,7 +976,133 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="38100"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'POCMA TS'!$A$7:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Day 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'POCMA TS'!$Y$7:$Y$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.90715456034953579</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.91616208663251053</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93290841999329088</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94847528916929547</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.93675417661097848</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.94495884773662553</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.952947539210384</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="132528000"/>
+        <c:axId val="132529536"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="132528000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="132529536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="132529536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.96000000000000008"/>
+          <c:min val="0.9"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="132528000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1044,103 +1175,37 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="PFEF SRC"/>
-      <sheetName val="PFEF T"/>
-      <sheetName val="PFEF C"/>
-      <sheetName val="PFEA SRC"/>
-      <sheetName val="PFEA T"/>
-      <sheetName val="PFEA C"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="7">
-          <cell r="B7" t="str">
-            <v>ALL</v>
-          </cell>
-          <cell r="U7">
-            <v>0.37723877925437943</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8" t="str">
-            <v>interested</v>
-          </cell>
-          <cell r="U8">
-            <v>0.50416661987288003</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9" t="str">
-            <v>tennis</v>
-          </cell>
-          <cell r="U9">
-            <v>0.58385827500163889</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10" t="str">
-            <v>tennis-arrangements</v>
-          </cell>
-          <cell r="U10">
-            <v>0.29386188653629097</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11" t="str">
-            <v>tennis-organising</v>
-          </cell>
-          <cell r="U11">
-            <v>0.57928848262966048</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12" t="str">
-            <v>urgency</v>
-          </cell>
-          <cell r="U12">
-            <v>0.57149971405294531</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13" t="str">
-            <v>work-logistics</v>
-          </cell>
-          <cell r="U13">
-            <v>0.73538675494728178</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14" t="str">
-            <v>work-pers</v>
-          </cell>
-          <cell r="U14">
-            <v>0.67835317926251881</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15" t="str">
-            <v>work-relevant</v>
-          </cell>
-          <cell r="U15">
-            <v>0.45285214433040366</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2912,7 +2977,7 @@
   </sheetPr>
   <dimension ref="A1:AC49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="W49" sqref="W49"/>
     </sheetView>
   </sheetViews>
@@ -3798,8 +3863,8 @@
   </sheetPr>
   <dimension ref="A1:AC35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:Y3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AF19" sqref="AF19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4391,7 +4456,7 @@
     <mergeCell ref="S4:U4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>